<commit_message>
manuali per kadaser 1 831-2
</commit_message>
<xml_diff>
--- a/831-2/4-Te-dhenat-per-kataster/regjistri/17-Regjistri-i-ndërrimeve-për-ndertesë-831-Muzeqine-legalizimi.xlsx
+++ b/831-2/4-Te-dhenat-per-kataster/regjistri/17-Regjistri-i-ndërrimeve-për-ndertesë-831-Muzeqine-legalizimi.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Ferizaj\Greme\Ingjinjerike\173-4-Greme-Ademi\4-Te-dhenat-per-kataster\regjistri\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shtime\Petroviq\ing\1018-2-Petrove-Vedati-leg\4-Te-dhenat-per-kataster\regjistri\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798246CE-C475-4EAD-BB9A-CA522ACB0FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760"/>
+    <workbookView xWindow="600" yWindow="90" windowWidth="27960" windowHeight="16110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet2!$A$1:$P$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet2!$A$1:$P$21</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -87,9 +87,6 @@
     <t>Pronari / Shfrytëzuesi                                                                      Emri (Emri i prindit) Mbiemri</t>
   </si>
   <si>
-    <t>Ferizaj</t>
-  </si>
-  <si>
     <t>Gjithsej:</t>
   </si>
   <si>
@@ -105,28 +102,31 @@
     <t>Kati 1</t>
   </si>
   <si>
-    <t>Rr. "Renosansa" Fsh. Greme - Ferizaj</t>
-  </si>
-  <si>
-    <t>GRABOC</t>
-  </si>
-  <si>
     <t>P+1</t>
   </si>
   <si>
-    <t>Greme</t>
-  </si>
-  <si>
-    <t>O-72217024-00173-4-___-0</t>
-  </si>
-  <si>
-    <t>Adem (Ilaz) Sejdiu</t>
+    <t>SHTIME</t>
+  </si>
+  <si>
+    <t>Vedat (Danush) Rashiti</t>
+  </si>
+  <si>
+    <t>O-72809066-01018-2-___-0</t>
+  </si>
+  <si>
+    <t>Petrovë</t>
+  </si>
+  <si>
+    <t>Rashitovit</t>
+  </si>
+  <si>
+    <t>Rr. " Fadil Rashiti"Fsh. Petrovë- SHTIME</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -477,34 +477,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -525,58 +519,49 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -602,13 +587,22 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="2"/>
-    <cellStyle name="Normal 3 2" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -703,9 +697,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -743,9 +737,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -780,7 +774,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -815,7 +809,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -988,405 +982,450 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q668"/>
+  <dimension ref="A1:P667"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScale="130" zoomScaleNormal="115" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="3" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.5703125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="14" style="4" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" style="4" customWidth="1"/>
-    <col min="13" max="14" width="8" style="4" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14" style="2" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="2" customWidth="1"/>
+    <col min="13" max="14" width="8" style="2" customWidth="1"/>
+    <col min="15" max="15" width="20.7109375" style="2" customWidth="1"/>
     <col min="16" max="16" width="6.85546875" style="2" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-    </row>
-    <row r="3" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+    </row>
+    <row r="3" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-    </row>
-    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+    </row>
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="21"/>
-    </row>
-    <row r="10" spans="1:17" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="19"/>
+    </row>
+    <row r="10" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="K10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L10" s="22" t="s">
+      <c r="L10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="10" t="s">
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="P10" s="9" t="s">
+      <c r="P10" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26">
+    <row r="11" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
         <v>1</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C11" s="23" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="11">
+        <v>86.09</v>
+      </c>
+      <c r="H11" s="23">
+        <v>86.09</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="13">
-        <v>86.06</v>
-      </c>
-      <c r="H11" s="23">
-        <v>72.03</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="23" t="s">
+      <c r="K11" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="23" t="s">
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="23">
+        <v>1175820376</v>
+      </c>
+      <c r="P11" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="39"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="L11" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="23">
-        <v>1004577058</v>
-      </c>
-      <c r="P11" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q11" s="6"/>
-    </row>
-    <row r="12" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="16">
-        <v>83.27</v>
-      </c>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="6"/>
-    </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="28"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="14">
+      <c r="G12" s="14">
+        <v>95.84</v>
+      </c>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="28"/>
+    </row>
+    <row r="13" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="12">
         <f>SUM(G11:G12)</f>
-        <v>169.32999999999998</v>
-      </c>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="31"/>
-    </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>181.93</v>
+      </c>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="16"/>
+    </row>
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P16" s="5"/>
-    </row>
-    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P17" s="5"/>
-    </row>
-    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="40"/>
+      <c r="P16" s="40"/>
+    </row>
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="40"/>
+    </row>
+    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+    </row>
+    <row r="19" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39" t="s">
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="41"/>
-    </row>
-    <row r="22" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="37"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="40"/>
-      <c r="O22" s="40"/>
-      <c r="P22" s="42"/>
-    </row>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="36"/>
+    </row>
+    <row r="21" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="32"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="37"/>
+    </row>
+    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1399,16 +1438,16 @@
     <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P35" s="4"/>
+    </row>
     <row r="36" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P36" s="5"/>
+      <c r="P36" s="4"/>
     </row>
     <row r="37" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P37" s="5"/>
-    </row>
-    <row r="38" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P38" s="5"/>
-    </row>
+      <c r="P37" s="4"/>
+    </row>
+    <row r="38" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1424,18 +1463,18 @@
     <row r="51" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P56" s="4"/>
+    </row>
     <row r="57" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P57" s="5"/>
+      <c r="P57" s="4"/>
     </row>
     <row r="58" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P58" s="5"/>
-    </row>
-    <row r="59" spans="16:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="P59" s="5"/>
-    </row>
+      <c r="P58" s="4"/>
+    </row>
+    <row r="59" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="60" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="62" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1443,274 +1482,270 @@
     <row r="64" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="16:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="16:16" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="16:16" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P77" s="4"/>
+    </row>
     <row r="78" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P78" s="5"/>
+      <c r="P78" s="4"/>
     </row>
     <row r="79" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P79" s="5"/>
-    </row>
-    <row r="80" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P80" s="5"/>
+      <c r="P79" s="4"/>
+    </row>
+    <row r="98" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P98" s="4"/>
     </row>
     <row r="99" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P99" s="5"/>
+      <c r="P99" s="4"/>
     </row>
     <row r="100" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P100" s="5"/>
-    </row>
-    <row r="101" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P101" s="5"/>
+      <c r="P100" s="4"/>
+    </row>
+    <row r="119" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P119" s="4"/>
     </row>
     <row r="120" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P120" s="5"/>
+      <c r="P120" s="4"/>
     </row>
     <row r="121" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P121" s="5"/>
-    </row>
-    <row r="122" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P122" s="5"/>
+      <c r="P121" s="4"/>
+    </row>
+    <row r="140" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P140" s="4"/>
     </row>
     <row r="141" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P141" s="5"/>
+      <c r="P141" s="4"/>
     </row>
     <row r="142" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P142" s="5"/>
-    </row>
-    <row r="143" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P143" s="5"/>
+      <c r="P142" s="4"/>
+    </row>
+    <row r="161" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P161" s="4"/>
     </row>
     <row r="162" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P162" s="5"/>
+      <c r="P162" s="4"/>
     </row>
     <row r="163" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P163" s="5"/>
-    </row>
-    <row r="164" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P164" s="5"/>
+      <c r="P163" s="4"/>
+    </row>
+    <row r="182" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P182" s="4"/>
     </row>
     <row r="183" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P183" s="5"/>
+      <c r="P183" s="4"/>
     </row>
     <row r="184" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P184" s="5"/>
-    </row>
-    <row r="185" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P185" s="5"/>
+      <c r="P184" s="4"/>
+    </row>
+    <row r="203" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P203" s="4"/>
     </row>
     <row r="204" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P204" s="5"/>
+      <c r="P204" s="4"/>
     </row>
     <row r="205" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P205" s="5"/>
-    </row>
-    <row r="206" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P206" s="5"/>
+      <c r="P205" s="4"/>
+    </row>
+    <row r="224" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P224" s="4"/>
     </row>
     <row r="225" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P225" s="5"/>
+      <c r="P225" s="4"/>
     </row>
     <row r="226" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P226" s="5"/>
-    </row>
-    <row r="227" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P227" s="5"/>
+      <c r="P226" s="4"/>
+    </row>
+    <row r="245" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P245" s="4"/>
     </row>
     <row r="246" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P246" s="5"/>
+      <c r="P246" s="4"/>
     </row>
     <row r="247" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P247" s="5"/>
-    </row>
-    <row r="248" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P248" s="5"/>
+      <c r="P247" s="4"/>
+    </row>
+    <row r="266" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P266" s="4"/>
     </row>
     <row r="267" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P267" s="5"/>
+      <c r="P267" s="4"/>
     </row>
     <row r="268" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P268" s="5"/>
-    </row>
-    <row r="269" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P269" s="5"/>
+      <c r="P268" s="4"/>
+    </row>
+    <row r="287" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P287" s="4"/>
     </row>
     <row r="288" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P288" s="5"/>
+      <c r="P288" s="4"/>
     </row>
     <row r="289" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P289" s="5"/>
-    </row>
-    <row r="290" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P290" s="5"/>
+      <c r="P289" s="4"/>
+    </row>
+    <row r="308" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P308" s="4"/>
     </row>
     <row r="309" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P309" s="5"/>
+      <c r="P309" s="4"/>
     </row>
     <row r="310" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P310" s="5"/>
-    </row>
-    <row r="311" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P311" s="5"/>
+      <c r="P310" s="4"/>
+    </row>
+    <row r="329" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P329" s="4"/>
     </row>
     <row r="330" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P330" s="5"/>
+      <c r="P330" s="4"/>
     </row>
     <row r="331" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P331" s="5"/>
-    </row>
-    <row r="332" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P332" s="5"/>
+      <c r="P331" s="4"/>
+    </row>
+    <row r="350" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P350" s="4"/>
     </row>
     <row r="351" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P351" s="5"/>
+      <c r="P351" s="4"/>
     </row>
     <row r="352" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P352" s="5"/>
-    </row>
-    <row r="353" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P353" s="5"/>
+      <c r="P352" s="4"/>
+    </row>
+    <row r="371" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P371" s="4"/>
     </row>
     <row r="372" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P372" s="5"/>
+      <c r="P372" s="4"/>
     </row>
     <row r="373" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P373" s="5"/>
-    </row>
-    <row r="374" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P374" s="5"/>
+      <c r="P373" s="4"/>
+    </row>
+    <row r="392" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P392" s="4"/>
     </row>
     <row r="393" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P393" s="5"/>
+      <c r="P393" s="4"/>
     </row>
     <row r="394" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P394" s="5"/>
-    </row>
-    <row r="395" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P395" s="5"/>
+      <c r="P394" s="4"/>
+    </row>
+    <row r="413" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P413" s="4"/>
     </row>
     <row r="414" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P414" s="5"/>
+      <c r="P414" s="4"/>
     </row>
     <row r="415" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P415" s="5"/>
-    </row>
-    <row r="416" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P416" s="5"/>
+      <c r="P415" s="4"/>
+    </row>
+    <row r="434" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P434" s="4"/>
     </row>
     <row r="435" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P435" s="5"/>
+      <c r="P435" s="4"/>
     </row>
     <row r="436" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P436" s="5"/>
-    </row>
-    <row r="437" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P437" s="5"/>
+      <c r="P436" s="4"/>
+    </row>
+    <row r="455" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P455" s="4"/>
     </row>
     <row r="456" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P456" s="5"/>
+      <c r="P456" s="4"/>
     </row>
     <row r="457" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P457" s="5"/>
-    </row>
-    <row r="458" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P458" s="5"/>
+      <c r="P457" s="4"/>
+    </row>
+    <row r="476" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P476" s="4"/>
     </row>
     <row r="477" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P477" s="5"/>
+      <c r="P477" s="4"/>
     </row>
     <row r="478" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P478" s="5"/>
-    </row>
-    <row r="479" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P479" s="5"/>
+      <c r="P478" s="4"/>
+    </row>
+    <row r="497" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P497" s="4"/>
     </row>
     <row r="498" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P498" s="5"/>
+      <c r="P498" s="4"/>
     </row>
     <row r="499" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P499" s="5"/>
-    </row>
-    <row r="500" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P500" s="5"/>
+      <c r="P499" s="4"/>
+    </row>
+    <row r="518" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P518" s="4"/>
     </row>
     <row r="519" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P519" s="5"/>
+      <c r="P519" s="4"/>
     </row>
     <row r="520" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P520" s="5"/>
-    </row>
-    <row r="521" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P521" s="5"/>
+      <c r="P520" s="4"/>
+    </row>
+    <row r="539" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P539" s="4"/>
     </row>
     <row r="540" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P540" s="5"/>
+      <c r="P540" s="4"/>
     </row>
     <row r="541" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P541" s="5"/>
-    </row>
-    <row r="542" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P542" s="5"/>
+      <c r="P541" s="4"/>
+    </row>
+    <row r="560" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P560" s="4"/>
     </row>
     <row r="561" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P561" s="5"/>
+      <c r="P561" s="4"/>
     </row>
     <row r="562" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P562" s="5"/>
-    </row>
-    <row r="563" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P563" s="5"/>
+      <c r="P562" s="4"/>
+    </row>
+    <row r="581" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P581" s="4"/>
     </row>
     <row r="582" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P582" s="5"/>
+      <c r="P582" s="4"/>
     </row>
     <row r="583" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P583" s="5"/>
-    </row>
-    <row r="584" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P584" s="5"/>
+      <c r="P583" s="4"/>
+    </row>
+    <row r="602" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P602" s="4"/>
     </row>
     <row r="603" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P603" s="5"/>
+      <c r="P603" s="4"/>
     </row>
     <row r="604" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P604" s="5"/>
-    </row>
-    <row r="605" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P605" s="5"/>
+      <c r="P604" s="4"/>
+    </row>
+    <row r="623" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P623" s="4"/>
     </row>
     <row r="624" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P624" s="5"/>
+      <c r="P624" s="4"/>
     </row>
     <row r="625" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P625" s="5"/>
-    </row>
-    <row r="626" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P626" s="5"/>
+      <c r="P625" s="4"/>
+    </row>
+    <row r="644" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P644" s="4"/>
     </row>
     <row r="645" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P645" s="5"/>
+      <c r="P645" s="4"/>
     </row>
     <row r="646" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P646" s="5"/>
-    </row>
-    <row r="647" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P647" s="5"/>
+      <c r="P646" s="4"/>
+    </row>
+    <row r="665" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P665" s="4"/>
     </row>
     <row r="666" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P666" s="5"/>
+      <c r="P666" s="4"/>
     </row>
     <row r="667" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P667" s="5"/>
-    </row>
-    <row r="668" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P668" s="5"/>
+      <c r="P667" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A21:D22"/>
-    <mergeCell ref="E21:H22"/>
-    <mergeCell ref="I21:P22"/>
     <mergeCell ref="A4:P8"/>
     <mergeCell ref="A1:P3"/>
     <mergeCell ref="A9:P9"/>
@@ -1727,6 +1762,9 @@
     <mergeCell ref="O11:O13"/>
     <mergeCell ref="P11:P13"/>
     <mergeCell ref="L11:N13"/>
+    <mergeCell ref="A20:D21"/>
+    <mergeCell ref="E20:H21"/>
+    <mergeCell ref="I20:P21"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1737,7 +1775,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>